<commit_message>
fixed incorrect micro usb part number. Added hyperlinks to bom
</commit_message>
<xml_diff>
--- a/doc/ecg_bom_charger.xlsx
+++ b/doc/ecg_bom_charger.xlsx
@@ -147,27 +147,12 @@
     <t>CAP CER 4.7UF 6.3V 20% X5R 0402</t>
   </si>
   <si>
-    <t>ED90502-ND</t>
-  </si>
-  <si>
     <t>Mill-Max</t>
   </si>
   <si>
-    <t>829-22-001-20-001101</t>
-  </si>
-  <si>
-    <t>HEADER 1 POS R/A SIP PCB</t>
-  </si>
-  <si>
-    <t>WM5409CT-ND</t>
-  </si>
-  <si>
     <t>Molex</t>
   </si>
   <si>
-    <t>CONN HEADER 3POS 1.2MM VERT WTB</t>
-  </si>
-  <si>
     <t>MF-NSMF150-2CT-ND</t>
   </si>
   <si>
@@ -190,6 +175,21 @@
   </si>
   <si>
     <t>LED ORANGE CLEAR 0805</t>
+  </si>
+  <si>
+    <t>WM1399CT-ND</t>
+  </si>
+  <si>
+    <t>CONN RCPT MICRO USB R/A SMD</t>
+  </si>
+  <si>
+    <t>HEADER 2 POS R/A SIP PCB</t>
+  </si>
+  <si>
+    <t>829-22-002-20-001101</t>
+  </si>
+  <si>
+    <t>ED90503-ND</t>
   </si>
 </sst>
 </file>
@@ -318,7 +318,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -404,6 +404,10 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="12">
     <cellStyle name="Explanatory Text" xfId="2" builtinId="53"/>
@@ -722,7 +726,7 @@
   <dimension ref="A1:L30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75"/>
@@ -805,7 +809,7 @@
       <c r="B4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="31" t="s">
         <v>24</v>
       </c>
       <c r="D4" s="13" t="s">
@@ -1007,29 +1011,29 @@
         <v>10</v>
       </c>
       <c r="C12" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="D12" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>43</v>
-      </c>
       <c r="E12" s="25" t="s">
-        <v>44</v>
+        <v>55</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="G12" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H12" s="13">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I12" s="22">
-        <v>8.7100000000000009</v>
+        <v>10.119999999999999</v>
       </c>
       <c r="J12" s="22">
         <f>H12*I12</f>
-        <v>17.420000000000002</v>
+        <v>10.119999999999999</v>
       </c>
     </row>
     <row r="13" spans="1:10">
@@ -1040,16 +1044,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="20" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E13" s="17">
-        <v>781710003</v>
+        <v>1050170001</v>
       </c>
       <c r="F13" s="17" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="G13" s="17" t="s">
         <v>11</v>
@@ -1058,11 +1062,11 @@
         <v>1</v>
       </c>
       <c r="I13" s="29">
-        <v>0.71</v>
+        <v>1</v>
       </c>
       <c r="J13" s="22">
         <f>H13*I13</f>
-        <v>0.71</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:10">
@@ -1085,16 +1089,16 @@
         <v>10</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D15" s="13" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="E15" s="25" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F15" s="25" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="G15" s="13" t="s">
         <v>11</v>
@@ -1129,17 +1133,17 @@
       <c r="B17" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="27" t="s">
-        <v>49</v>
+      <c r="C17" s="32" t="s">
+        <v>44</v>
       </c>
       <c r="D17" s="16" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E17" s="25" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F17" s="25" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="G17" s="16" t="s">
         <v>11</v>
@@ -1181,7 +1185,7 @@
       </c>
       <c r="J19" s="22">
         <f>SUM(J4:J17)</f>
-        <v>20.49</v>
+        <v>13.48</v>
       </c>
     </row>
     <row r="20" spans="1:12">
@@ -1226,7 +1230,7 @@
       </c>
       <c r="J22" s="30">
         <f>SUM(H4:H17)</f>
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:12">
@@ -1286,8 +1290,19 @@
       <c r="J30" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C4" r:id="rId1"/>
+    <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="C7" r:id="rId3"/>
+    <hyperlink ref="C8" r:id="rId4"/>
+    <hyperlink ref="C10" r:id="rId5"/>
+    <hyperlink ref="C13" r:id="rId6"/>
+    <hyperlink ref="C15" r:id="rId7"/>
+    <hyperlink ref="C17" r:id="rId8"/>
+    <hyperlink ref="C12" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId10"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>